<commit_message>
Update with Assignment 2 Start
</commit_message>
<xml_diff>
--- a/output/portfolio_performance.xlsx
+++ b/output/portfolio_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcw/Documents/SMT Master/EPFL/Finance/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65DCC99-674B-DC42-B84E-67B5A57AA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654DB760-D3BD-5C47-9023-9B83C9B31266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="28000" windowHeight="16800" xr2:uid="{2F94277C-2214-EB46-A08E-E90DAA2E3A14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Portfolio</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Volatility</t>
+  </si>
+  <si>
+    <t>Portfolio volatility</t>
+  </si>
+  <si>
+    <t>Portfolio return</t>
+  </si>
+  <si>
+    <t>Portfolio Sharpe ratio</t>
+  </si>
+  <si>
+    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
     <numFmt numFmtId="169" formatCode="0.000%"/>
     <numFmt numFmtId="175" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,6 +191,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -281,8 +304,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -325,6 +351,7 @@
     <xf numFmtId="169" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="5" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -333,9 +360,12 @@
     </xf>
     <xf numFmtId="175" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="175" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -654,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F402C1B1-73F7-454F-BC3F-2E01AD8FB737}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,607 +697,652 @@
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>6.7799999999999999E-2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>0.1145</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="10" t="s">
+      <c r="D3" s="2"/>
+      <c r="F3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>6.7799999999999999E-2</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="12">
         <v>0.1145</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>0.2261</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>0.46610000000000001</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="2"/>
+      <c r="F4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="14">
         <v>0.2261</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="14">
         <v>0.46610000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>-0.45429999999999998</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>-0.60129999999999995</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="2"/>
+      <c r="F5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>-0.45429999999999998</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="14">
         <v>-0.60129999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>0.50260000000000005</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>0.7621</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="2"/>
+      <c r="F6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="14">
         <v>0.50260000000000005</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="14">
         <v>0.7621</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>7.8700000000000006E-2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>0.1384</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="2"/>
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="14">
         <v>7.8700000000000006E-2</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="14">
         <v>0.1384</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="22">
         <v>4.7350000000000003E-2</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="F10" s="16" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="23">
         <v>4.7350000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="24">
         <v>7.9060000000000005E-2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="F11" s="15" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="F11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="23">
         <v>7.9060000000000005E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="22">
         <v>1.8610000000000002E-2</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="F12" s="15" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="23">
         <v>1.8610000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="24">
         <v>4.0719999999999999E-2</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="F13" s="15" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="23">
         <v>4.0719999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="22">
         <v>6.5170000000000006E-2</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="F14" s="15" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="23">
         <v>6.5170000000000006E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="4">
         <v>4.7300000000000002E-2</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="12">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="12">
         <v>0.1145</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="11">
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="7">
         <v>0.13009999999999999</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>0.47320000000000001</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>6.5199999999999994E-2</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="14">
         <v>0.13009999999999999</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="14">
         <v>0.47320000000000001</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="13">
         <v>6.5199999999999994E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5">
         <v>-4.2900000000000001E-2</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <v>1.8599999999999998E-2</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="14">
         <v>-4.2900000000000001E-2</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="14">
         <v>-0.11890000000000001</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="13">
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="7">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>7.9100000000000004E-2</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="14">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="14">
         <v>0.16209999999999999</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="13">
         <v>7.9100000000000004E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="5">
         <v>-0.1807</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <v>0.1363</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>-4.07E-2</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="14">
         <v>-0.1807</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="14">
         <v>0.1363</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="13">
         <v>-4.07E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="G24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="G25" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="25">
         <v>185</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="26">
         <v>185</v>
       </c>
+      <c r="G26" s="42">
+        <v>0.22</v>
+      </c>
+      <c r="H26" s="42">
+        <v>0.132766</v>
+      </c>
+      <c r="I26" s="41">
+        <v>1.506408</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="27">
         <v>0.11451</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="27">
         <v>0.44006400000000001</v>
       </c>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="37"/>
+      <c r="G27" s="42">
+        <v>0.24</v>
+      </c>
+      <c r="H27" s="42">
+        <v>0.14611299999999999</v>
+      </c>
+      <c r="I27" s="41">
+        <v>1.5056879999999999</v>
+      </c>
+      <c r="J27" s="37"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="28">
         <v>-0.244423</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="29">
         <v>0.155693</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="37"/>
+      <c r="G28" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="H28" s="42">
+        <v>0.120778</v>
+      </c>
+      <c r="I28" s="41">
+        <v>1.4903390000000001</v>
+      </c>
+      <c r="J28" s="37"/>
+      <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="19">
+      <c r="A29" s="20">
         <v>0.25</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="30">
         <v>6.7505999999999997E-2</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="30">
         <v>0.34715000000000001</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="37"/>
+      <c r="G29" s="42">
+        <v>0.26</v>
+      </c>
+      <c r="H29" s="42">
+        <v>0.161386</v>
+      </c>
+      <c r="I29" s="41">
+        <v>1.4871160000000001</v>
+      </c>
+      <c r="J29" s="37"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="18">
+      <c r="A30" s="19">
         <v>0.5</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="28">
         <v>0.111135</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="29">
         <v>0.42035499999999998</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="37"/>
+      <c r="G30" s="42">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H30" s="42">
+        <v>0.17802899999999999</v>
+      </c>
+      <c r="I30" s="41">
+        <v>1.4604349999999999</v>
+      </c>
+      <c r="J30" s="37"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
+      <c r="A31" s="6">
         <v>0.75</v>
       </c>
-      <c r="B31" s="30">
+      <c r="B31" s="31">
         <v>0.167964</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="27">
         <v>0.50837399999999999</v>
       </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="37"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="38"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="28">
         <v>0.45264300000000002</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="29">
         <v>1.2439480000000001</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="37"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F33" s="36"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="37"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="38"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="37"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="5">
         <v>1</v>
       </c>
-      <c r="C35" s="33">
+      <c r="C35" s="35">
         <v>0.106325</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="37"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="38"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="34">
+      <c r="B36" s="36">
         <v>0.106325</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="7">
         <v>1</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="37"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F37" s="36"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F38" s="36"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="15">
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="J35:J36"/>
     <mergeCell ref="K35:K36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="G24:I24"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="K27:K28"/>
     <mergeCell ref="J29:J30"/>
@@ -1275,25 +1350,10 @@
     <mergeCell ref="J31:J32"/>
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="J33:J34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A24:C24"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>